<commit_message>
Edited download files from homepage
</commit_message>
<xml_diff>
--- a/doc/cost-study-data.xlsx
+++ b/doc/cost-study-data.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="cost-study&gt;total-medical-cost" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="cost-study&gt;demographics" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="costs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="demographics" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>